<commit_message>
PSP und Zeitplan 30.01.2012
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitplan.xlsx
+++ b/Dokumente/Zeitplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Arbeitspakete</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Pufferzeit</t>
+  </si>
+  <si>
+    <t>Zeitgemäß abgeschlossen</t>
   </si>
 </sst>
 </file>
@@ -198,7 +201,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -235,6 +238,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="40">
     <border>
@@ -735,7 +744,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -800,6 +809,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
@@ -1210,7 +1223,7 @@
       <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AU27" sqref="AU27"/>
+      <selection pane="bottomRight" activeCell="E38" sqref="E38:E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.42578125" defaultRowHeight="15"/>
@@ -1242,6 +1255,10 @@
       <c r="AH2" s="55"/>
       <c r="AI2" t="s">
         <v>42</v>
+      </c>
+      <c r="AM2" s="65"/>
+      <c r="AN2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:44" ht="15.75" thickBot="1">
@@ -1290,10 +1307,10 @@
       <c r="AK4" s="3"/>
       <c r="AL4" s="3"/>
       <c r="AM4" s="14"/>
-      <c r="AN4" s="95" t="s">
+      <c r="AN4" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="AO4" s="96"/>
+      <c r="AO4" s="100"/>
       <c r="AP4" s="3"/>
       <c r="AQ4" s="23"/>
       <c r="AR4" s="23"/>
@@ -1355,13 +1372,13 @@
       <c r="V5" s="22">
         <v>22</v>
       </c>
-      <c r="W5" s="82" t="s">
+      <c r="W5" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="X5" s="83"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="83"/>
-      <c r="AA5" s="84"/>
+      <c r="X5" s="87"/>
+      <c r="Y5" s="87"/>
+      <c r="Z5" s="87"/>
+      <c r="AA5" s="88"/>
       <c r="AB5" s="30">
         <v>5</v>
       </c>
@@ -1412,11 +1429,11 @@
     </row>
     <row r="6" spans="2:44" ht="15.75" customHeight="1" thickTop="1">
       <c r="B6" s="5"/>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="97" t="s">
+      <c r="D6" s="67"/>
+      <c r="E6" s="101" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="52"/>
@@ -1436,13 +1453,13 @@
       <c r="T6" s="6"/>
       <c r="U6" s="53"/>
       <c r="V6" s="54"/>
-      <c r="W6" s="85" t="s">
+      <c r="W6" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="X6" s="86"/>
-      <c r="Y6" s="86"/>
-      <c r="Z6" s="86"/>
-      <c r="AA6" s="87"/>
+      <c r="X6" s="90"/>
+      <c r="Y6" s="90"/>
+      <c r="Z6" s="90"/>
+      <c r="AA6" s="91"/>
       <c r="AB6" s="6"/>
       <c r="AC6" s="2"/>
       <c r="AD6" s="11"/>
@@ -1462,12 +1479,12 @@
     </row>
     <row r="7" spans="2:44">
       <c r="B7" s="5"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="81"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="85"/>
       <c r="F7" s="40"/>
       <c r="G7" s="41"/>
-      <c r="H7" s="42"/>
+      <c r="H7" s="63"/>
       <c r="I7" s="4"/>
       <c r="J7" s="1"/>
       <c r="K7" s="12"/>
@@ -1482,11 +1499,11 @@
       <c r="T7" s="4"/>
       <c r="U7" s="55"/>
       <c r="V7" s="56"/>
-      <c r="W7" s="88"/>
-      <c r="X7" s="89"/>
-      <c r="Y7" s="89"/>
-      <c r="Z7" s="89"/>
-      <c r="AA7" s="90"/>
+      <c r="W7" s="92"/>
+      <c r="X7" s="93"/>
+      <c r="Y7" s="93"/>
+      <c r="Z7" s="93"/>
+      <c r="AA7" s="94"/>
       <c r="AB7" s="4"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="12"/>
@@ -1505,9 +1522,9 @@
     </row>
     <row r="8" spans="2:44">
       <c r="B8" s="5"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="80" t="s">
+      <c r="C8" s="66"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="84" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="4"/>
@@ -1527,11 +1544,11 @@
       <c r="T8" s="4"/>
       <c r="U8" s="55"/>
       <c r="V8" s="56"/>
-      <c r="W8" s="88"/>
-      <c r="X8" s="89"/>
-      <c r="Y8" s="89"/>
-      <c r="Z8" s="89"/>
-      <c r="AA8" s="90"/>
+      <c r="W8" s="92"/>
+      <c r="X8" s="93"/>
+      <c r="Y8" s="93"/>
+      <c r="Z8" s="93"/>
+      <c r="AA8" s="94"/>
       <c r="AB8" s="4"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="12"/>
@@ -1550,9 +1567,9 @@
     </row>
     <row r="9" spans="2:44">
       <c r="B9" s="5"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="81"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="85"/>
       <c r="F9" s="4"/>
       <c r="G9" s="41"/>
       <c r="H9" s="42"/>
@@ -1570,11 +1587,11 @@
       <c r="T9" s="4"/>
       <c r="U9" s="55"/>
       <c r="V9" s="56"/>
-      <c r="W9" s="88"/>
-      <c r="X9" s="89"/>
-      <c r="Y9" s="89"/>
-      <c r="Z9" s="89"/>
-      <c r="AA9" s="90"/>
+      <c r="W9" s="92"/>
+      <c r="X9" s="93"/>
+      <c r="Y9" s="93"/>
+      <c r="Z9" s="93"/>
+      <c r="AA9" s="94"/>
       <c r="AB9" s="4"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="12"/>
@@ -1593,9 +1610,9 @@
     </row>
     <row r="10" spans="2:44">
       <c r="B10" s="5"/>
-      <c r="C10" s="62"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="98" t="s">
+      <c r="C10" s="66"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="102" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="4"/>
@@ -1615,11 +1632,11 @@
       <c r="T10" s="4"/>
       <c r="U10" s="55"/>
       <c r="V10" s="56"/>
-      <c r="W10" s="88"/>
-      <c r="X10" s="89"/>
-      <c r="Y10" s="89"/>
-      <c r="Z10" s="89"/>
-      <c r="AA10" s="90"/>
+      <c r="W10" s="92"/>
+      <c r="X10" s="93"/>
+      <c r="Y10" s="93"/>
+      <c r="Z10" s="93"/>
+      <c r="AA10" s="94"/>
       <c r="AB10" s="4"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="12"/>
@@ -1638,16 +1655,16 @@
     </row>
     <row r="11" spans="2:44">
       <c r="B11" s="5"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="99"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="103"/>
       <c r="F11" s="4"/>
       <c r="G11" s="1"/>
       <c r="H11" s="12"/>
       <c r="I11" s="4"/>
       <c r="J11" s="41"/>
       <c r="K11" s="42"/>
-      <c r="L11" s="40"/>
+      <c r="L11" s="64"/>
       <c r="M11" s="1"/>
       <c r="N11" s="12"/>
       <c r="O11" s="4"/>
@@ -1658,11 +1675,11 @@
       <c r="T11" s="4"/>
       <c r="U11" s="55"/>
       <c r="V11" s="56"/>
-      <c r="W11" s="88"/>
-      <c r="X11" s="89"/>
-      <c r="Y11" s="89"/>
-      <c r="Z11" s="89"/>
-      <c r="AA11" s="90"/>
+      <c r="W11" s="92"/>
+      <c r="X11" s="93"/>
+      <c r="Y11" s="93"/>
+      <c r="Z11" s="93"/>
+      <c r="AA11" s="94"/>
       <c r="AB11" s="4"/>
       <c r="AC11" s="1"/>
       <c r="AD11" s="12"/>
@@ -1681,9 +1698,9 @@
     </row>
     <row r="12" spans="2:44">
       <c r="B12" s="5"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="80" t="s">
+      <c r="C12" s="66"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="84" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="4"/>
@@ -1703,11 +1720,11 @@
       <c r="T12" s="4"/>
       <c r="U12" s="55"/>
       <c r="V12" s="56"/>
-      <c r="W12" s="88"/>
-      <c r="X12" s="89"/>
-      <c r="Y12" s="89"/>
-      <c r="Z12" s="89"/>
-      <c r="AA12" s="90"/>
+      <c r="W12" s="92"/>
+      <c r="X12" s="93"/>
+      <c r="Y12" s="93"/>
+      <c r="Z12" s="93"/>
+      <c r="AA12" s="94"/>
       <c r="AB12" s="4"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="12"/>
@@ -1726,9 +1743,9 @@
     </row>
     <row r="13" spans="2:44">
       <c r="B13" s="5"/>
-      <c r="C13" s="62"/>
-      <c r="D13" s="63"/>
-      <c r="E13" s="81"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="67"/>
+      <c r="E13" s="85"/>
       <c r="F13" s="4"/>
       <c r="G13" s="1"/>
       <c r="H13" s="12"/>
@@ -1746,11 +1763,11 @@
       <c r="T13" s="4"/>
       <c r="U13" s="55"/>
       <c r="V13" s="56"/>
-      <c r="W13" s="88"/>
-      <c r="X13" s="89"/>
-      <c r="Y13" s="89"/>
-      <c r="Z13" s="89"/>
-      <c r="AA13" s="90"/>
+      <c r="W13" s="92"/>
+      <c r="X13" s="93"/>
+      <c r="Y13" s="93"/>
+      <c r="Z13" s="93"/>
+      <c r="AA13" s="94"/>
       <c r="AB13" s="4"/>
       <c r="AC13" s="1"/>
       <c r="AD13" s="12"/>
@@ -1769,9 +1786,9 @@
     </row>
     <row r="14" spans="2:44">
       <c r="B14" s="5"/>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="98" t="s">
+      <c r="C14" s="66"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="102" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="4"/>
@@ -1791,11 +1808,11 @@
       <c r="T14" s="4"/>
       <c r="U14" s="55"/>
       <c r="V14" s="56"/>
-      <c r="W14" s="88"/>
-      <c r="X14" s="89"/>
-      <c r="Y14" s="89"/>
-      <c r="Z14" s="89"/>
-      <c r="AA14" s="90"/>
+      <c r="W14" s="92"/>
+      <c r="X14" s="93"/>
+      <c r="Y14" s="93"/>
+      <c r="Z14" s="93"/>
+      <c r="AA14" s="94"/>
       <c r="AB14" s="4"/>
       <c r="AC14" s="1"/>
       <c r="AD14" s="12"/>
@@ -1814,9 +1831,9 @@
     </row>
     <row r="15" spans="2:44">
       <c r="B15" s="5"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="99"/>
+      <c r="C15" s="66"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="103"/>
       <c r="F15" s="4"/>
       <c r="G15" s="1"/>
       <c r="H15" s="12"/>
@@ -1834,11 +1851,11 @@
       <c r="T15" s="4"/>
       <c r="U15" s="55"/>
       <c r="V15" s="56"/>
-      <c r="W15" s="88"/>
-      <c r="X15" s="89"/>
-      <c r="Y15" s="89"/>
-      <c r="Z15" s="89"/>
-      <c r="AA15" s="90"/>
+      <c r="W15" s="92"/>
+      <c r="X15" s="93"/>
+      <c r="Y15" s="93"/>
+      <c r="Z15" s="93"/>
+      <c r="AA15" s="94"/>
       <c r="AB15" s="4"/>
       <c r="AC15" s="1"/>
       <c r="AD15" s="12"/>
@@ -1857,9 +1874,9 @@
     </row>
     <row r="16" spans="2:44">
       <c r="B16" s="5"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="98" t="s">
+      <c r="C16" s="66"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="102" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="4"/>
@@ -1879,11 +1896,11 @@
       <c r="T16" s="4"/>
       <c r="U16" s="55"/>
       <c r="V16" s="56"/>
-      <c r="W16" s="88"/>
-      <c r="X16" s="89"/>
-      <c r="Y16" s="89"/>
-      <c r="Z16" s="89"/>
-      <c r="AA16" s="90"/>
+      <c r="W16" s="92"/>
+      <c r="X16" s="93"/>
+      <c r="Y16" s="93"/>
+      <c r="Z16" s="93"/>
+      <c r="AA16" s="94"/>
       <c r="AB16" s="4"/>
       <c r="AC16" s="1"/>
       <c r="AD16" s="12"/>
@@ -1902,16 +1919,16 @@
     </row>
     <row r="17" spans="2:42">
       <c r="B17" s="5"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="99"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="103"/>
       <c r="F17" s="4"/>
       <c r="G17" s="1"/>
       <c r="H17" s="12"/>
       <c r="I17" s="4"/>
       <c r="J17" s="1"/>
       <c r="K17" s="42"/>
-      <c r="L17" s="4"/>
+      <c r="L17" s="40"/>
       <c r="M17" s="1"/>
       <c r="N17" s="12"/>
       <c r="O17" s="4"/>
@@ -1922,11 +1939,11 @@
       <c r="T17" s="4"/>
       <c r="U17" s="55"/>
       <c r="V17" s="56"/>
-      <c r="W17" s="88"/>
-      <c r="X17" s="89"/>
-      <c r="Y17" s="89"/>
-      <c r="Z17" s="89"/>
-      <c r="AA17" s="90"/>
+      <c r="W17" s="92"/>
+      <c r="X17" s="93"/>
+      <c r="Y17" s="93"/>
+      <c r="Z17" s="93"/>
+      <c r="AA17" s="94"/>
       <c r="AB17" s="4"/>
       <c r="AC17" s="1"/>
       <c r="AD17" s="12"/>
@@ -1945,9 +1962,9 @@
     </row>
     <row r="18" spans="2:42">
       <c r="B18" s="5"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="98" t="s">
+      <c r="C18" s="66"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="102" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="4"/>
@@ -1967,11 +1984,11 @@
       <c r="T18" s="4"/>
       <c r="U18" s="55"/>
       <c r="V18" s="56"/>
-      <c r="W18" s="88"/>
-      <c r="X18" s="89"/>
-      <c r="Y18" s="89"/>
-      <c r="Z18" s="89"/>
-      <c r="AA18" s="90"/>
+      <c r="W18" s="92"/>
+      <c r="X18" s="93"/>
+      <c r="Y18" s="93"/>
+      <c r="Z18" s="93"/>
+      <c r="AA18" s="94"/>
       <c r="AB18" s="4"/>
       <c r="AC18" s="1"/>
       <c r="AD18" s="12"/>
@@ -1990,16 +2007,16 @@
     </row>
     <row r="19" spans="2:42">
       <c r="B19" s="5"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="99"/>
+      <c r="C19" s="66"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="103"/>
       <c r="F19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="12"/>
       <c r="I19" s="4"/>
       <c r="J19" s="1"/>
       <c r="K19" s="42"/>
-      <c r="L19" s="4"/>
+      <c r="L19" s="62"/>
       <c r="M19" s="1"/>
       <c r="N19" s="12"/>
       <c r="O19" s="4"/>
@@ -2010,11 +2027,11 @@
       <c r="T19" s="4"/>
       <c r="U19" s="55"/>
       <c r="V19" s="56"/>
-      <c r="W19" s="88"/>
-      <c r="X19" s="89"/>
-      <c r="Y19" s="89"/>
-      <c r="Z19" s="89"/>
-      <c r="AA19" s="90"/>
+      <c r="W19" s="92"/>
+      <c r="X19" s="93"/>
+      <c r="Y19" s="93"/>
+      <c r="Z19" s="93"/>
+      <c r="AA19" s="94"/>
       <c r="AB19" s="4"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="12"/>
@@ -2033,9 +2050,9 @@
     </row>
     <row r="20" spans="2:42">
       <c r="B20" s="5"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="80" t="s">
+      <c r="C20" s="66"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="84" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="4"/>
@@ -2055,11 +2072,11 @@
       <c r="T20" s="4"/>
       <c r="U20" s="55"/>
       <c r="V20" s="56"/>
-      <c r="W20" s="88"/>
-      <c r="X20" s="89"/>
-      <c r="Y20" s="89"/>
-      <c r="Z20" s="89"/>
-      <c r="AA20" s="90"/>
+      <c r="W20" s="92"/>
+      <c r="X20" s="93"/>
+      <c r="Y20" s="93"/>
+      <c r="Z20" s="93"/>
+      <c r="AA20" s="94"/>
       <c r="AB20" s="4"/>
       <c r="AC20" s="1"/>
       <c r="AD20" s="12"/>
@@ -2078,9 +2095,9 @@
     </row>
     <row r="21" spans="2:42" ht="15.75" thickBot="1">
       <c r="B21" s="5"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="81"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="85"/>
       <c r="F21" s="4"/>
       <c r="G21" s="1"/>
       <c r="H21" s="12"/>
@@ -2098,11 +2115,11 @@
       <c r="T21" s="4"/>
       <c r="U21" s="55"/>
       <c r="V21" s="56"/>
-      <c r="W21" s="88"/>
-      <c r="X21" s="89"/>
-      <c r="Y21" s="89"/>
-      <c r="Z21" s="89"/>
-      <c r="AA21" s="90"/>
+      <c r="W21" s="92"/>
+      <c r="X21" s="93"/>
+      <c r="Y21" s="93"/>
+      <c r="Z21" s="93"/>
+      <c r="AA21" s="94"/>
       <c r="AB21" s="4"/>
       <c r="AC21" s="1"/>
       <c r="AD21" s="12"/>
@@ -2121,11 +2138,11 @@
     </row>
     <row r="22" spans="2:42" ht="15.75" thickTop="1">
       <c r="B22" s="5"/>
-      <c r="C22" s="66" t="s">
+      <c r="C22" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="67"/>
-      <c r="E22" s="78" t="s">
+      <c r="D22" s="71"/>
+      <c r="E22" s="82" t="s">
         <v>17</v>
       </c>
       <c r="F22" s="4"/>
@@ -2145,11 +2162,11 @@
       <c r="T22" s="4"/>
       <c r="U22" s="55"/>
       <c r="V22" s="56"/>
-      <c r="W22" s="88"/>
-      <c r="X22" s="89"/>
-      <c r="Y22" s="89"/>
-      <c r="Z22" s="89"/>
-      <c r="AA22" s="90"/>
+      <c r="W22" s="92"/>
+      <c r="X22" s="93"/>
+      <c r="Y22" s="93"/>
+      <c r="Z22" s="93"/>
+      <c r="AA22" s="94"/>
       <c r="AB22" s="4"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="12"/>
@@ -2168,16 +2185,16 @@
     </row>
     <row r="23" spans="2:42">
       <c r="B23" s="5"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="79"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="83"/>
       <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" s="12"/>
       <c r="I23" s="4"/>
       <c r="J23" s="1"/>
       <c r="K23" s="12"/>
-      <c r="L23" s="4"/>
+      <c r="L23" s="40"/>
       <c r="M23" s="1"/>
       <c r="N23" s="12"/>
       <c r="O23" s="4"/>
@@ -2188,11 +2205,11 @@
       <c r="T23" s="4"/>
       <c r="U23" s="55"/>
       <c r="V23" s="56"/>
-      <c r="W23" s="88"/>
-      <c r="X23" s="89"/>
-      <c r="Y23" s="89"/>
-      <c r="Z23" s="89"/>
-      <c r="AA23" s="90"/>
+      <c r="W23" s="92"/>
+      <c r="X23" s="93"/>
+      <c r="Y23" s="93"/>
+      <c r="Z23" s="93"/>
+      <c r="AA23" s="94"/>
       <c r="AB23" s="4"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="12"/>
@@ -2211,9 +2228,9 @@
     </row>
     <row r="24" spans="2:42">
       <c r="B24" s="5"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="78" t="s">
+      <c r="C24" s="72"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="82" t="s">
         <v>7</v>
       </c>
       <c r="F24" s="4"/>
@@ -2233,11 +2250,11 @@
       <c r="T24" s="4"/>
       <c r="U24" s="55"/>
       <c r="V24" s="56"/>
-      <c r="W24" s="88"/>
-      <c r="X24" s="89"/>
-      <c r="Y24" s="89"/>
-      <c r="Z24" s="89"/>
-      <c r="AA24" s="90"/>
+      <c r="W24" s="92"/>
+      <c r="X24" s="93"/>
+      <c r="Y24" s="93"/>
+      <c r="Z24" s="93"/>
+      <c r="AA24" s="94"/>
       <c r="AB24" s="4"/>
       <c r="AC24" s="1"/>
       <c r="AD24" s="12"/>
@@ -2256,9 +2273,9 @@
     </row>
     <row r="25" spans="2:42">
       <c r="B25" s="5"/>
-      <c r="C25" s="68"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="79"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="83"/>
       <c r="F25" s="4"/>
       <c r="G25" s="1"/>
       <c r="H25" s="44"/>
@@ -2276,11 +2293,11 @@
       <c r="T25" s="4"/>
       <c r="U25" s="55"/>
       <c r="V25" s="56"/>
-      <c r="W25" s="88"/>
-      <c r="X25" s="89"/>
-      <c r="Y25" s="89"/>
-      <c r="Z25" s="89"/>
-      <c r="AA25" s="90"/>
+      <c r="W25" s="92"/>
+      <c r="X25" s="93"/>
+      <c r="Y25" s="93"/>
+      <c r="Z25" s="93"/>
+      <c r="AA25" s="94"/>
       <c r="AB25" s="4"/>
       <c r="AC25" s="1"/>
       <c r="AD25" s="12"/>
@@ -2299,9 +2316,9 @@
     </row>
     <row r="26" spans="2:42">
       <c r="B26" s="5"/>
-      <c r="C26" s="68"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="78" t="s">
+      <c r="C26" s="72"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="82" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="4"/>
@@ -2321,11 +2338,11 @@
       <c r="T26" s="4"/>
       <c r="U26" s="55"/>
       <c r="V26" s="56"/>
-      <c r="W26" s="88"/>
-      <c r="X26" s="89"/>
-      <c r="Y26" s="89"/>
-      <c r="Z26" s="89"/>
-      <c r="AA26" s="90"/>
+      <c r="W26" s="92"/>
+      <c r="X26" s="93"/>
+      <c r="Y26" s="93"/>
+      <c r="Z26" s="93"/>
+      <c r="AA26" s="94"/>
       <c r="AB26" s="4"/>
       <c r="AC26" s="1"/>
       <c r="AD26" s="12"/>
@@ -2344,9 +2361,9 @@
     </row>
     <row r="27" spans="2:42" ht="15.75" customHeight="1">
       <c r="B27" s="5"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="79"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="83"/>
       <c r="F27" s="4"/>
       <c r="G27" s="1"/>
       <c r="H27" s="12"/>
@@ -2364,11 +2381,11 @@
       <c r="T27" s="4"/>
       <c r="U27" s="55"/>
       <c r="V27" s="56"/>
-      <c r="W27" s="88"/>
-      <c r="X27" s="89"/>
-      <c r="Y27" s="89"/>
-      <c r="Z27" s="89"/>
-      <c r="AA27" s="90"/>
+      <c r="W27" s="92"/>
+      <c r="X27" s="93"/>
+      <c r="Y27" s="93"/>
+      <c r="Z27" s="93"/>
+      <c r="AA27" s="94"/>
       <c r="AB27" s="4"/>
       <c r="AC27" s="1"/>
       <c r="AD27" s="12"/>
@@ -2387,9 +2404,9 @@
     </row>
     <row r="28" spans="2:42">
       <c r="B28" s="5"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="78" t="s">
+      <c r="C28" s="72"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="82" t="s">
         <v>30</v>
       </c>
       <c r="F28" s="33"/>
@@ -2409,11 +2426,11 @@
       <c r="T28" s="4"/>
       <c r="U28" s="55"/>
       <c r="V28" s="56"/>
-      <c r="W28" s="88"/>
-      <c r="X28" s="89"/>
-      <c r="Y28" s="89"/>
-      <c r="Z28" s="89"/>
-      <c r="AA28" s="90"/>
+      <c r="W28" s="92"/>
+      <c r="X28" s="93"/>
+      <c r="Y28" s="93"/>
+      <c r="Z28" s="93"/>
+      <c r="AA28" s="94"/>
       <c r="AB28" s="4"/>
       <c r="AC28" s="1"/>
       <c r="AD28" s="12"/>
@@ -2432,9 +2449,9 @@
     </row>
     <row r="29" spans="2:42">
       <c r="B29" s="5"/>
-      <c r="C29" s="68"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="79"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="83"/>
       <c r="F29" s="34"/>
       <c r="G29" s="2"/>
       <c r="H29" s="11"/>
@@ -2452,11 +2469,11 @@
       <c r="T29" s="6"/>
       <c r="U29" s="53"/>
       <c r="V29" s="54"/>
-      <c r="W29" s="88"/>
-      <c r="X29" s="89"/>
-      <c r="Y29" s="89"/>
-      <c r="Z29" s="89"/>
-      <c r="AA29" s="90"/>
+      <c r="W29" s="92"/>
+      <c r="X29" s="93"/>
+      <c r="Y29" s="93"/>
+      <c r="Z29" s="93"/>
+      <c r="AA29" s="94"/>
       <c r="AB29" s="4"/>
       <c r="AC29" s="1"/>
       <c r="AD29" s="12"/>
@@ -2475,9 +2492,9 @@
     </row>
     <row r="30" spans="2:42">
       <c r="B30" s="5"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="78" t="s">
+      <c r="C30" s="72"/>
+      <c r="D30" s="73"/>
+      <c r="E30" s="82" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="33"/>
@@ -2497,11 +2514,11 @@
       <c r="T30" s="4"/>
       <c r="U30" s="55"/>
       <c r="V30" s="56"/>
-      <c r="W30" s="88"/>
-      <c r="X30" s="89"/>
-      <c r="Y30" s="89"/>
-      <c r="Z30" s="89"/>
-      <c r="AA30" s="90"/>
+      <c r="W30" s="92"/>
+      <c r="X30" s="93"/>
+      <c r="Y30" s="93"/>
+      <c r="Z30" s="93"/>
+      <c r="AA30" s="94"/>
       <c r="AB30" s="4"/>
       <c r="AC30" s="1"/>
       <c r="AD30" s="12"/>
@@ -2520,9 +2537,9 @@
     </row>
     <row r="31" spans="2:42" ht="15.75" customHeight="1">
       <c r="B31" s="5"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="79"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="73"/>
+      <c r="E31" s="83"/>
       <c r="F31" s="33"/>
       <c r="G31" s="1"/>
       <c r="H31" s="12"/>
@@ -2540,11 +2557,11 @@
       <c r="T31" s="4"/>
       <c r="U31" s="55"/>
       <c r="V31" s="56"/>
-      <c r="W31" s="88"/>
-      <c r="X31" s="89"/>
-      <c r="Y31" s="89"/>
-      <c r="Z31" s="89"/>
-      <c r="AA31" s="90"/>
+      <c r="W31" s="92"/>
+      <c r="X31" s="93"/>
+      <c r="Y31" s="93"/>
+      <c r="Z31" s="93"/>
+      <c r="AA31" s="94"/>
       <c r="AB31" s="4"/>
       <c r="AC31" s="1"/>
       <c r="AD31" s="12"/>
@@ -2563,9 +2580,9 @@
     </row>
     <row r="32" spans="2:42" ht="15.75" customHeight="1" thickBot="1">
       <c r="B32" s="5"/>
-      <c r="C32" s="68"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="78" t="s">
+      <c r="C32" s="72"/>
+      <c r="D32" s="73"/>
+      <c r="E32" s="82" t="s">
         <v>18</v>
       </c>
       <c r="F32" s="33"/>
@@ -2585,11 +2602,11 @@
       <c r="T32" s="4"/>
       <c r="U32" s="55"/>
       <c r="V32" s="56"/>
-      <c r="W32" s="88"/>
-      <c r="X32" s="89"/>
-      <c r="Y32" s="89"/>
-      <c r="Z32" s="89"/>
-      <c r="AA32" s="90"/>
+      <c r="W32" s="92"/>
+      <c r="X32" s="93"/>
+      <c r="Y32" s="93"/>
+      <c r="Z32" s="93"/>
+      <c r="AA32" s="94"/>
       <c r="AB32" s="4"/>
       <c r="AC32" s="1"/>
       <c r="AD32" s="12"/>
@@ -2608,9 +2625,9 @@
     </row>
     <row r="33" spans="2:42" ht="15.75" thickTop="1">
       <c r="B33" s="5"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="79"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="73"/>
+      <c r="E33" s="83"/>
       <c r="F33" s="33"/>
       <c r="G33" s="1"/>
       <c r="H33" s="12"/>
@@ -2628,13 +2645,13 @@
       <c r="T33" s="4"/>
       <c r="U33" s="55"/>
       <c r="V33" s="56"/>
-      <c r="W33" s="85" t="s">
+      <c r="W33" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="X33" s="86"/>
-      <c r="Y33" s="86"/>
-      <c r="Z33" s="86"/>
-      <c r="AA33" s="87"/>
+      <c r="X33" s="90"/>
+      <c r="Y33" s="90"/>
+      <c r="Z33" s="90"/>
+      <c r="AA33" s="91"/>
       <c r="AB33" s="4"/>
       <c r="AC33" s="1"/>
       <c r="AD33" s="12"/>
@@ -2653,9 +2670,9 @@
     </row>
     <row r="34" spans="2:42">
       <c r="B34" s="5"/>
-      <c r="C34" s="68"/>
-      <c r="D34" s="69"/>
-      <c r="E34" s="78" t="s">
+      <c r="C34" s="72"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="82" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="33"/>
@@ -2675,11 +2692,11 @@
       <c r="T34" s="4"/>
       <c r="U34" s="55"/>
       <c r="V34" s="56"/>
-      <c r="W34" s="88"/>
-      <c r="X34" s="89"/>
-      <c r="Y34" s="89"/>
-      <c r="Z34" s="89"/>
-      <c r="AA34" s="90"/>
+      <c r="W34" s="92"/>
+      <c r="X34" s="93"/>
+      <c r="Y34" s="93"/>
+      <c r="Z34" s="93"/>
+      <c r="AA34" s="94"/>
       <c r="AB34" s="4"/>
       <c r="AC34" s="1"/>
       <c r="AD34" s="12"/>
@@ -2698,9 +2715,9 @@
     </row>
     <row r="35" spans="2:42">
       <c r="B35" s="5"/>
-      <c r="C35" s="68"/>
-      <c r="D35" s="69"/>
-      <c r="E35" s="79"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="73"/>
+      <c r="E35" s="83"/>
       <c r="F35" s="33"/>
       <c r="G35" s="1"/>
       <c r="H35" s="12"/>
@@ -2718,11 +2735,11 @@
       <c r="T35" s="4"/>
       <c r="U35" s="55"/>
       <c r="V35" s="56"/>
-      <c r="W35" s="88"/>
-      <c r="X35" s="89"/>
-      <c r="Y35" s="89"/>
-      <c r="Z35" s="89"/>
-      <c r="AA35" s="90"/>
+      <c r="W35" s="92"/>
+      <c r="X35" s="93"/>
+      <c r="Y35" s="93"/>
+      <c r="Z35" s="93"/>
+      <c r="AA35" s="94"/>
       <c r="AB35" s="4"/>
       <c r="AC35" s="1"/>
       <c r="AD35" s="12"/>
@@ -2741,9 +2758,9 @@
     </row>
     <row r="36" spans="2:42">
       <c r="B36" s="5"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="78" t="s">
+      <c r="C36" s="72"/>
+      <c r="D36" s="73"/>
+      <c r="E36" s="82" t="s">
         <v>19</v>
       </c>
       <c r="F36" s="33"/>
@@ -2763,11 +2780,11 @@
       <c r="T36" s="4"/>
       <c r="U36" s="55"/>
       <c r="V36" s="56"/>
-      <c r="W36" s="88"/>
-      <c r="X36" s="89"/>
-      <c r="Y36" s="89"/>
-      <c r="Z36" s="89"/>
-      <c r="AA36" s="90"/>
+      <c r="W36" s="92"/>
+      <c r="X36" s="93"/>
+      <c r="Y36" s="93"/>
+      <c r="Z36" s="93"/>
+      <c r="AA36" s="94"/>
       <c r="AB36" s="4"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="12"/>
@@ -2786,9 +2803,9 @@
     </row>
     <row r="37" spans="2:42" ht="15.75" thickBot="1">
       <c r="B37" s="5"/>
-      <c r="C37" s="70"/>
-      <c r="D37" s="71"/>
-      <c r="E37" s="79"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="83"/>
       <c r="F37" s="33"/>
       <c r="G37" s="1"/>
       <c r="H37" s="12"/>
@@ -2806,11 +2823,11 @@
       <c r="T37" s="4"/>
       <c r="U37" s="55"/>
       <c r="V37" s="56"/>
-      <c r="W37" s="88"/>
-      <c r="X37" s="89"/>
-      <c r="Y37" s="89"/>
-      <c r="Z37" s="89"/>
-      <c r="AA37" s="90"/>
+      <c r="W37" s="92"/>
+      <c r="X37" s="93"/>
+      <c r="Y37" s="93"/>
+      <c r="Z37" s="93"/>
+      <c r="AA37" s="94"/>
       <c r="AB37" s="4"/>
       <c r="AC37" s="1"/>
       <c r="AD37" s="12"/>
@@ -2828,11 +2845,11 @@
       <c r="AP37" s="12"/>
     </row>
     <row r="38" spans="2:42" ht="15.75" thickTop="1">
-      <c r="C38" s="66" t="s">
+      <c r="C38" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="67"/>
-      <c r="E38" s="78" t="s">
+      <c r="D38" s="71"/>
+      <c r="E38" s="82" t="s">
         <v>20</v>
       </c>
       <c r="F38" s="33"/>
@@ -2852,11 +2869,11 @@
       <c r="T38" s="4"/>
       <c r="U38" s="55"/>
       <c r="V38" s="56"/>
-      <c r="W38" s="88"/>
-      <c r="X38" s="89"/>
-      <c r="Y38" s="89"/>
-      <c r="Z38" s="89"/>
-      <c r="AA38" s="90"/>
+      <c r="W38" s="92"/>
+      <c r="X38" s="93"/>
+      <c r="Y38" s="93"/>
+      <c r="Z38" s="93"/>
+      <c r="AA38" s="94"/>
       <c r="AB38" s="4"/>
       <c r="AC38" s="1"/>
       <c r="AD38" s="12"/>
@@ -2874,9 +2891,9 @@
       <c r="AP38" s="12"/>
     </row>
     <row r="39" spans="2:42">
-      <c r="C39" s="68"/>
-      <c r="D39" s="69"/>
-      <c r="E39" s="79"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="73"/>
+      <c r="E39" s="83"/>
       <c r="F39" s="4"/>
       <c r="G39" s="1"/>
       <c r="H39" s="12"/>
@@ -2894,11 +2911,11 @@
       <c r="T39" s="4"/>
       <c r="U39" s="55"/>
       <c r="V39" s="56"/>
-      <c r="W39" s="88"/>
-      <c r="X39" s="89"/>
-      <c r="Y39" s="89"/>
-      <c r="Z39" s="89"/>
-      <c r="AA39" s="90"/>
+      <c r="W39" s="92"/>
+      <c r="X39" s="93"/>
+      <c r="Y39" s="93"/>
+      <c r="Z39" s="93"/>
+      <c r="AA39" s="94"/>
       <c r="AB39" s="4"/>
       <c r="AC39" s="1"/>
       <c r="AD39" s="12"/>
@@ -2916,9 +2933,9 @@
       <c r="AP39" s="12"/>
     </row>
     <row r="40" spans="2:42">
-      <c r="C40" s="68"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="78" t="s">
+      <c r="C40" s="72"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="82" t="s">
         <v>34</v>
       </c>
       <c r="F40" s="33"/>
@@ -2938,11 +2955,11 @@
       <c r="T40" s="61"/>
       <c r="U40" s="55"/>
       <c r="V40" s="56"/>
-      <c r="W40" s="88"/>
-      <c r="X40" s="89"/>
-      <c r="Y40" s="89"/>
-      <c r="Z40" s="89"/>
-      <c r="AA40" s="90"/>
+      <c r="W40" s="92"/>
+      <c r="X40" s="93"/>
+      <c r="Y40" s="93"/>
+      <c r="Z40" s="93"/>
+      <c r="AA40" s="94"/>
       <c r="AB40" s="4"/>
       <c r="AC40" s="1"/>
       <c r="AD40" s="12"/>
@@ -2960,9 +2977,9 @@
       <c r="AP40" s="12"/>
     </row>
     <row r="41" spans="2:42">
-      <c r="C41" s="68"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="79"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="83"/>
       <c r="F41" s="33"/>
       <c r="G41" s="1"/>
       <c r="H41" s="12"/>
@@ -2980,11 +2997,11 @@
       <c r="T41" s="4"/>
       <c r="U41" s="55"/>
       <c r="V41" s="56"/>
-      <c r="W41" s="88"/>
-      <c r="X41" s="89"/>
-      <c r="Y41" s="89"/>
-      <c r="Z41" s="89"/>
-      <c r="AA41" s="90"/>
+      <c r="W41" s="92"/>
+      <c r="X41" s="93"/>
+      <c r="Y41" s="93"/>
+      <c r="Z41" s="93"/>
+      <c r="AA41" s="94"/>
       <c r="AB41" s="4"/>
       <c r="AC41" s="1"/>
       <c r="AD41" s="12"/>
@@ -3002,9 +3019,9 @@
       <c r="AP41" s="12"/>
     </row>
     <row r="42" spans="2:42">
-      <c r="C42" s="68"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="78" t="s">
+      <c r="C42" s="72"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="82" t="s">
         <v>22</v>
       </c>
       <c r="F42" s="33"/>
@@ -3024,11 +3041,11 @@
       <c r="T42" s="61"/>
       <c r="U42" s="55"/>
       <c r="V42" s="56"/>
-      <c r="W42" s="88"/>
-      <c r="X42" s="89"/>
-      <c r="Y42" s="89"/>
-      <c r="Z42" s="89"/>
-      <c r="AA42" s="90"/>
+      <c r="W42" s="92"/>
+      <c r="X42" s="93"/>
+      <c r="Y42" s="93"/>
+      <c r="Z42" s="93"/>
+      <c r="AA42" s="94"/>
       <c r="AB42" s="4"/>
       <c r="AC42" s="1"/>
       <c r="AD42" s="12"/>
@@ -3046,9 +3063,9 @@
       <c r="AP42" s="12"/>
     </row>
     <row r="43" spans="2:42">
-      <c r="C43" s="68"/>
-      <c r="D43" s="69"/>
-      <c r="E43" s="79"/>
+      <c r="C43" s="72"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="83"/>
       <c r="F43" s="33"/>
       <c r="G43" s="1"/>
       <c r="H43" s="12"/>
@@ -3066,11 +3083,11 @@
       <c r="T43" s="4"/>
       <c r="U43" s="55"/>
       <c r="V43" s="56"/>
-      <c r="W43" s="88"/>
-      <c r="X43" s="89"/>
-      <c r="Y43" s="89"/>
-      <c r="Z43" s="89"/>
-      <c r="AA43" s="90"/>
+      <c r="W43" s="92"/>
+      <c r="X43" s="93"/>
+      <c r="Y43" s="93"/>
+      <c r="Z43" s="93"/>
+      <c r="AA43" s="94"/>
       <c r="AB43" s="4"/>
       <c r="AC43" s="1"/>
       <c r="AD43" s="12"/>
@@ -3088,9 +3105,9 @@
       <c r="AP43" s="12"/>
     </row>
     <row r="44" spans="2:42">
-      <c r="C44" s="68"/>
-      <c r="D44" s="69"/>
-      <c r="E44" s="78" t="s">
+      <c r="C44" s="72"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="82" t="s">
         <v>29</v>
       </c>
       <c r="F44" s="33"/>
@@ -3110,11 +3127,11 @@
       <c r="T44" s="4"/>
       <c r="U44" s="55"/>
       <c r="V44" s="56"/>
-      <c r="W44" s="88"/>
-      <c r="X44" s="89"/>
-      <c r="Y44" s="89"/>
-      <c r="Z44" s="89"/>
-      <c r="AA44" s="90"/>
+      <c r="W44" s="92"/>
+      <c r="X44" s="93"/>
+      <c r="Y44" s="93"/>
+      <c r="Z44" s="93"/>
+      <c r="AA44" s="94"/>
       <c r="AB44" s="37"/>
       <c r="AC44" s="35"/>
       <c r="AD44" s="12"/>
@@ -3132,9 +3149,9 @@
       <c r="AP44" s="12"/>
     </row>
     <row r="45" spans="2:42">
-      <c r="C45" s="68"/>
-      <c r="D45" s="69"/>
-      <c r="E45" s="79"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="73"/>
+      <c r="E45" s="83"/>
       <c r="F45" s="33"/>
       <c r="G45" s="1"/>
       <c r="H45" s="12"/>
@@ -3152,11 +3169,11 @@
       <c r="T45" s="4"/>
       <c r="U45" s="55"/>
       <c r="V45" s="56"/>
-      <c r="W45" s="88"/>
-      <c r="X45" s="89"/>
-      <c r="Y45" s="89"/>
-      <c r="Z45" s="89"/>
-      <c r="AA45" s="90"/>
+      <c r="W45" s="92"/>
+      <c r="X45" s="93"/>
+      <c r="Y45" s="93"/>
+      <c r="Z45" s="93"/>
+      <c r="AA45" s="94"/>
       <c r="AB45" s="4"/>
       <c r="AC45" s="1"/>
       <c r="AD45" s="12"/>
@@ -3174,9 +3191,9 @@
       <c r="AP45" s="12"/>
     </row>
     <row r="46" spans="2:42">
-      <c r="C46" s="68"/>
-      <c r="D46" s="69"/>
-      <c r="E46" s="78" t="s">
+      <c r="C46" s="72"/>
+      <c r="D46" s="73"/>
+      <c r="E46" s="82" t="s">
         <v>21</v>
       </c>
       <c r="F46" s="33"/>
@@ -3196,11 +3213,11 @@
       <c r="T46" s="4"/>
       <c r="U46" s="55"/>
       <c r="V46" s="56"/>
-      <c r="W46" s="88"/>
-      <c r="X46" s="89"/>
-      <c r="Y46" s="89"/>
-      <c r="Z46" s="89"/>
-      <c r="AA46" s="90"/>
+      <c r="W46" s="92"/>
+      <c r="X46" s="93"/>
+      <c r="Y46" s="93"/>
+      <c r="Z46" s="93"/>
+      <c r="AA46" s="94"/>
       <c r="AB46" s="4"/>
       <c r="AC46" s="1"/>
       <c r="AD46" s="36"/>
@@ -3218,9 +3235,9 @@
       <c r="AP46" s="12"/>
     </row>
     <row r="47" spans="2:42">
-      <c r="C47" s="68"/>
-      <c r="D47" s="69"/>
-      <c r="E47" s="79"/>
+      <c r="C47" s="72"/>
+      <c r="D47" s="73"/>
+      <c r="E47" s="83"/>
       <c r="F47" s="4"/>
       <c r="G47" s="1"/>
       <c r="H47" s="12"/>
@@ -3238,11 +3255,11 @@
       <c r="T47" s="4"/>
       <c r="U47" s="55"/>
       <c r="V47" s="56"/>
-      <c r="W47" s="88"/>
-      <c r="X47" s="89"/>
-      <c r="Y47" s="89"/>
-      <c r="Z47" s="89"/>
-      <c r="AA47" s="90"/>
+      <c r="W47" s="92"/>
+      <c r="X47" s="93"/>
+      <c r="Y47" s="93"/>
+      <c r="Z47" s="93"/>
+      <c r="AA47" s="94"/>
       <c r="AB47" s="4"/>
       <c r="AC47" s="1"/>
       <c r="AD47" s="12"/>
@@ -3260,9 +3277,9 @@
       <c r="AP47" s="12"/>
     </row>
     <row r="48" spans="2:42">
-      <c r="C48" s="68"/>
-      <c r="D48" s="69"/>
-      <c r="E48" s="78" t="s">
+      <c r="C48" s="72"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="82" t="s">
         <v>23</v>
       </c>
       <c r="F48" s="33"/>
@@ -3282,11 +3299,11 @@
       <c r="T48" s="4"/>
       <c r="U48" s="55"/>
       <c r="V48" s="56"/>
-      <c r="W48" s="88"/>
-      <c r="X48" s="89"/>
-      <c r="Y48" s="89"/>
-      <c r="Z48" s="89"/>
-      <c r="AA48" s="90"/>
+      <c r="W48" s="92"/>
+      <c r="X48" s="93"/>
+      <c r="Y48" s="93"/>
+      <c r="Z48" s="93"/>
+      <c r="AA48" s="94"/>
       <c r="AB48" s="4"/>
       <c r="AC48" s="1"/>
       <c r="AD48" s="12"/>
@@ -3304,9 +3321,9 @@
       <c r="AP48" s="12"/>
     </row>
     <row r="49" spans="3:42">
-      <c r="C49" s="68"/>
-      <c r="D49" s="69"/>
-      <c r="E49" s="79"/>
+      <c r="C49" s="72"/>
+      <c r="D49" s="73"/>
+      <c r="E49" s="83"/>
       <c r="F49" s="4"/>
       <c r="G49" s="1"/>
       <c r="H49" s="12"/>
@@ -3324,11 +3341,11 @@
       <c r="T49" s="4"/>
       <c r="U49" s="55"/>
       <c r="V49" s="56"/>
-      <c r="W49" s="88"/>
-      <c r="X49" s="89"/>
-      <c r="Y49" s="89"/>
-      <c r="Z49" s="89"/>
-      <c r="AA49" s="90"/>
+      <c r="W49" s="92"/>
+      <c r="X49" s="93"/>
+      <c r="Y49" s="93"/>
+      <c r="Z49" s="93"/>
+      <c r="AA49" s="94"/>
       <c r="AB49" s="4"/>
       <c r="AC49" s="1"/>
       <c r="AD49" s="12"/>
@@ -3346,9 +3363,9 @@
       <c r="AP49" s="12"/>
     </row>
     <row r="50" spans="3:42">
-      <c r="C50" s="68"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="78" t="s">
+      <c r="C50" s="72"/>
+      <c r="D50" s="73"/>
+      <c r="E50" s="82" t="s">
         <v>24</v>
       </c>
       <c r="F50" s="33"/>
@@ -3368,11 +3385,11 @@
       <c r="T50" s="4"/>
       <c r="U50" s="55"/>
       <c r="V50" s="56"/>
-      <c r="W50" s="88"/>
-      <c r="X50" s="89"/>
-      <c r="Y50" s="89"/>
-      <c r="Z50" s="89"/>
-      <c r="AA50" s="90"/>
+      <c r="W50" s="92"/>
+      <c r="X50" s="93"/>
+      <c r="Y50" s="93"/>
+      <c r="Z50" s="93"/>
+      <c r="AA50" s="94"/>
       <c r="AB50" s="4"/>
       <c r="AC50" s="1"/>
       <c r="AD50" s="12"/>
@@ -3390,9 +3407,9 @@
       <c r="AP50" s="12"/>
     </row>
     <row r="51" spans="3:42" ht="15.75" thickBot="1">
-      <c r="C51" s="70"/>
-      <c r="D51" s="71"/>
-      <c r="E51" s="79"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="75"/>
+      <c r="E51" s="83"/>
       <c r="F51" s="4"/>
       <c r="G51" s="1"/>
       <c r="H51" s="12"/>
@@ -3410,11 +3427,11 @@
       <c r="T51" s="4"/>
       <c r="U51" s="55"/>
       <c r="V51" s="56"/>
-      <c r="W51" s="88"/>
-      <c r="X51" s="89"/>
-      <c r="Y51" s="89"/>
-      <c r="Z51" s="89"/>
-      <c r="AA51" s="90"/>
+      <c r="W51" s="92"/>
+      <c r="X51" s="93"/>
+      <c r="Y51" s="93"/>
+      <c r="Z51" s="93"/>
+      <c r="AA51" s="94"/>
       <c r="AB51" s="4"/>
       <c r="AC51" s="1"/>
       <c r="AD51" s="12"/>
@@ -3432,11 +3449,11 @@
       <c r="AP51" s="12"/>
     </row>
     <row r="52" spans="3:42" ht="15.75" thickTop="1">
-      <c r="C52" s="72" t="s">
+      <c r="C52" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="D52" s="73"/>
-      <c r="E52" s="78" t="s">
+      <c r="D52" s="77"/>
+      <c r="E52" s="82" t="s">
         <v>25</v>
       </c>
       <c r="F52" s="33"/>
@@ -3456,11 +3473,11 @@
       <c r="T52" s="4"/>
       <c r="U52" s="55"/>
       <c r="V52" s="56"/>
-      <c r="W52" s="88"/>
-      <c r="X52" s="89"/>
-      <c r="Y52" s="89"/>
-      <c r="Z52" s="89"/>
-      <c r="AA52" s="90"/>
+      <c r="W52" s="92"/>
+      <c r="X52" s="93"/>
+      <c r="Y52" s="93"/>
+      <c r="Z52" s="93"/>
+      <c r="AA52" s="94"/>
       <c r="AB52" s="4"/>
       <c r="AC52" s="1"/>
       <c r="AD52" s="12"/>
@@ -3478,9 +3495,9 @@
       <c r="AP52" s="12"/>
     </row>
     <row r="53" spans="3:42">
-      <c r="C53" s="74"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="79"/>
+      <c r="C53" s="78"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="83"/>
       <c r="F53" s="4"/>
       <c r="G53" s="1"/>
       <c r="H53" s="12"/>
@@ -3498,11 +3515,11 @@
       <c r="T53" s="4"/>
       <c r="U53" s="55"/>
       <c r="V53" s="56"/>
-      <c r="W53" s="88"/>
-      <c r="X53" s="89"/>
-      <c r="Y53" s="89"/>
-      <c r="Z53" s="89"/>
-      <c r="AA53" s="90"/>
+      <c r="W53" s="92"/>
+      <c r="X53" s="93"/>
+      <c r="Y53" s="93"/>
+      <c r="Z53" s="93"/>
+      <c r="AA53" s="94"/>
       <c r="AB53" s="4"/>
       <c r="AC53" s="1"/>
       <c r="AD53" s="12"/>
@@ -3520,9 +3537,9 @@
       <c r="AP53" s="12"/>
     </row>
     <row r="54" spans="3:42">
-      <c r="C54" s="74"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="78" t="s">
+      <c r="C54" s="78"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="82" t="s">
         <v>26</v>
       </c>
       <c r="F54" s="33"/>
@@ -3542,11 +3559,11 @@
       <c r="T54" s="4"/>
       <c r="U54" s="55"/>
       <c r="V54" s="56"/>
-      <c r="W54" s="88"/>
-      <c r="X54" s="89"/>
-      <c r="Y54" s="89"/>
-      <c r="Z54" s="89"/>
-      <c r="AA54" s="90"/>
+      <c r="W54" s="92"/>
+      <c r="X54" s="93"/>
+      <c r="Y54" s="93"/>
+      <c r="Z54" s="93"/>
+      <c r="AA54" s="94"/>
       <c r="AB54" s="4"/>
       <c r="AC54" s="1"/>
       <c r="AD54" s="12"/>
@@ -3564,9 +3581,9 @@
       <c r="AP54" s="12"/>
     </row>
     <row r="55" spans="3:42">
-      <c r="C55" s="74"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="79"/>
+      <c r="C55" s="78"/>
+      <c r="D55" s="79"/>
+      <c r="E55" s="83"/>
       <c r="F55" s="4"/>
       <c r="G55" s="1"/>
       <c r="H55" s="12"/>
@@ -3584,11 +3601,11 @@
       <c r="T55" s="4"/>
       <c r="U55" s="55"/>
       <c r="V55" s="56"/>
-      <c r="W55" s="88"/>
-      <c r="X55" s="89"/>
-      <c r="Y55" s="89"/>
-      <c r="Z55" s="89"/>
-      <c r="AA55" s="90"/>
+      <c r="W55" s="92"/>
+      <c r="X55" s="93"/>
+      <c r="Y55" s="93"/>
+      <c r="Z55" s="93"/>
+      <c r="AA55" s="94"/>
       <c r="AB55" s="48"/>
       <c r="AC55" s="46"/>
       <c r="AD55" s="47"/>
@@ -3606,9 +3623,9 @@
       <c r="AP55" s="47"/>
     </row>
     <row r="56" spans="3:42">
-      <c r="C56" s="74"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="78" t="s">
+      <c r="C56" s="78"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="82" t="s">
         <v>27</v>
       </c>
       <c r="F56" s="33"/>
@@ -3628,11 +3645,11 @@
       <c r="T56" s="4"/>
       <c r="U56" s="55"/>
       <c r="V56" s="56"/>
-      <c r="W56" s="88"/>
-      <c r="X56" s="89"/>
-      <c r="Y56" s="89"/>
-      <c r="Z56" s="89"/>
-      <c r="AA56" s="90"/>
+      <c r="W56" s="92"/>
+      <c r="X56" s="93"/>
+      <c r="Y56" s="93"/>
+      <c r="Z56" s="93"/>
+      <c r="AA56" s="94"/>
       <c r="AB56" s="4"/>
       <c r="AC56" s="1"/>
       <c r="AD56" s="12"/>
@@ -3650,9 +3667,9 @@
       <c r="AP56" s="36"/>
     </row>
     <row r="57" spans="3:42">
-      <c r="C57" s="74"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="79"/>
+      <c r="C57" s="78"/>
+      <c r="D57" s="79"/>
+      <c r="E57" s="83"/>
       <c r="F57" s="33"/>
       <c r="G57" s="1"/>
       <c r="H57" s="12"/>
@@ -3670,11 +3687,11 @@
       <c r="T57" s="4"/>
       <c r="U57" s="55"/>
       <c r="V57" s="56"/>
-      <c r="W57" s="88"/>
-      <c r="X57" s="89"/>
-      <c r="Y57" s="89"/>
-      <c r="Z57" s="89"/>
-      <c r="AA57" s="90"/>
+      <c r="W57" s="92"/>
+      <c r="X57" s="93"/>
+      <c r="Y57" s="93"/>
+      <c r="Z57" s="93"/>
+      <c r="AA57" s="94"/>
       <c r="AB57" s="4"/>
       <c r="AC57" s="1"/>
       <c r="AD57" s="12"/>
@@ -3692,9 +3709,9 @@
       <c r="AP57" s="12"/>
     </row>
     <row r="58" spans="3:42">
-      <c r="C58" s="74"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="78" t="s">
+      <c r="C58" s="78"/>
+      <c r="D58" s="79"/>
+      <c r="E58" s="82" t="s">
         <v>28</v>
       </c>
       <c r="F58" s="34"/>
@@ -3714,11 +3731,11 @@
       <c r="T58" s="6"/>
       <c r="U58" s="53"/>
       <c r="V58" s="54"/>
-      <c r="W58" s="88"/>
-      <c r="X58" s="89"/>
-      <c r="Y58" s="89"/>
-      <c r="Z58" s="89"/>
-      <c r="AA58" s="90"/>
+      <c r="W58" s="92"/>
+      <c r="X58" s="93"/>
+      <c r="Y58" s="93"/>
+      <c r="Z58" s="93"/>
+      <c r="AA58" s="94"/>
       <c r="AB58" s="4"/>
       <c r="AC58" s="1"/>
       <c r="AD58" s="12"/>
@@ -3736,9 +3753,9 @@
       <c r="AP58" s="50"/>
     </row>
     <row r="59" spans="3:42" ht="15.75" thickBot="1">
-      <c r="C59" s="76"/>
-      <c r="D59" s="77"/>
-      <c r="E59" s="94"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="98"/>
       <c r="F59" s="45"/>
       <c r="G59" s="27"/>
       <c r="H59" s="28"/>
@@ -3756,11 +3773,11 @@
       <c r="T59" s="29"/>
       <c r="U59" s="57"/>
       <c r="V59" s="58"/>
-      <c r="W59" s="91"/>
-      <c r="X59" s="92"/>
-      <c r="Y59" s="92"/>
-      <c r="Z59" s="92"/>
-      <c r="AA59" s="93"/>
+      <c r="W59" s="95"/>
+      <c r="X59" s="96"/>
+      <c r="Y59" s="96"/>
+      <c r="Z59" s="96"/>
+      <c r="AA59" s="97"/>
       <c r="AB59" s="45"/>
       <c r="AC59" s="27"/>
       <c r="AD59" s="28"/>

</xml_diff>